<commit_message>
- Converted the costs of aidres and the danish catalogue to EUR-2025 - Add more info on the calculation of the extra data - Removed rows with zero production
</commit_message>
<xml_diff>
--- a/input_data/extra_data/Mopo_Data_Collection_CH_NO_UK.xlsx
+++ b/input_data/extra_data/Mopo_Data_Collection_CH_NO_UK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vitoresearch-my.sharepoint.com/personal/hans_vandeput_vito_be/Documents/Mopo/mopo_repo/input_data/extra_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="376" documentId="8_{64D5985E-4681-4148-A659-EEB7E7B1CE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17097719-196E-47AD-B4CF-1FEE22C147BA}"/>
+  <xr:revisionPtr revIDLastSave="378" documentId="8_{64D5985E-4681-4148-A659-EEB7E7B1CE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A802911-DBE4-4D8E-BCC1-929C9DA298AF}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{03389423-7521-48F9-AC41-5D13B8A33616}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03389423-7521-48F9-AC41-5D13B8A33616}"/>
   </bookViews>
   <sheets>
     <sheet name="extra_data" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -410,15 +410,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -439,9 +434,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -479,7 +474,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -585,7 +580,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -727,7 +722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -739,7 +734,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H66" sqref="H66"/>
+      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,7 +742,7 @@
     <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
     <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -800,7 +795,7 @@
       <c r="C2" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>74</v>
       </c>
       <c r="E2" t="s">
@@ -833,7 +828,7 @@
       <c r="C3" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>74</v>
       </c>
       <c r="E3" t="s">
@@ -866,7 +861,7 @@
       <c r="C4" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
         <v>74</v>
       </c>
       <c r="E4" t="s">
@@ -899,7 +894,7 @@
       <c r="C5" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" t="s">
         <v>74</v>
       </c>
       <c r="E5" t="s">
@@ -932,7 +927,7 @@
       <c r="C6" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" t="s">
         <v>74</v>
       </c>
       <c r="E6" t="s">
@@ -965,7 +960,7 @@
       <c r="C7" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" t="s">
         <v>74</v>
       </c>
       <c r="E7" t="s">
@@ -998,7 +993,7 @@
       <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" t="s">
         <v>74</v>
       </c>
       <c r="E8" t="s">
@@ -1031,7 +1026,7 @@
       <c r="C9" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" t="s">
         <v>74</v>
       </c>
       <c r="E9" t="s">
@@ -1064,7 +1059,7 @@
       <c r="C10" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
         <v>78</v>
       </c>
       <c r="E10" t="s">
@@ -1096,7 +1091,7 @@
       <c r="C11" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
         <v>78</v>
       </c>
       <c r="E11" t="s">
@@ -1128,7 +1123,7 @@
       <c r="C12" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
         <v>78</v>
       </c>
       <c r="E12" t="s">
@@ -1160,7 +1155,7 @@
       <c r="C13" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" t="s">
         <v>78</v>
       </c>
       <c r="E13" t="s">
@@ -1192,7 +1187,7 @@
       <c r="C14" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" t="s">
         <v>78</v>
       </c>
       <c r="E14" t="s">
@@ -1224,7 +1219,7 @@
       <c r="C15" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" t="s">
         <v>78</v>
       </c>
       <c r="E15" t="s">
@@ -1256,7 +1251,7 @@
       <c r="C16" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" t="s">
         <v>78</v>
       </c>
       <c r="E16" t="s">
@@ -1288,7 +1283,7 @@
       <c r="C17" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" t="s">
         <v>78</v>
       </c>
       <c r="E17" t="s">
@@ -1784,7 +1779,7 @@
       <c r="C34" t="s">
         <v>85</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" t="s">
         <v>54</v>
       </c>
       <c r="E34" t="s">
@@ -1816,7 +1811,7 @@
       <c r="C35" t="s">
         <v>85</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" t="s">
         <v>54</v>
       </c>
       <c r="E35" t="s">
@@ -1848,7 +1843,7 @@
       <c r="C36" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" t="s">
         <v>54</v>
       </c>
       <c r="E36" t="s">
@@ -1880,7 +1875,7 @@
       <c r="C37" t="s">
         <v>85</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" t="s">
         <v>54</v>
       </c>
       <c r="E37" t="s">
@@ -1912,7 +1907,7 @@
       <c r="C38" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" t="s">
         <v>54</v>
       </c>
       <c r="E38" t="s">
@@ -1944,7 +1939,7 @@
       <c r="C39" t="s">
         <v>85</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" t="s">
         <v>54</v>
       </c>
       <c r="E39" t="s">
@@ -1976,7 +1971,7 @@
       <c r="C40" t="s">
         <v>85</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" t="s">
         <v>54</v>
       </c>
       <c r="E40" t="s">
@@ -2008,7 +2003,7 @@
       <c r="C41" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" t="s">
         <v>54</v>
       </c>
       <c r="E41" t="s">
@@ -2040,7 +2035,7 @@
       <c r="C42" t="s">
         <v>85</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" t="s">
         <v>55</v>
       </c>
       <c r="E42" t="s">
@@ -2072,7 +2067,7 @@
       <c r="C43" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" t="s">
         <v>55</v>
       </c>
       <c r="E43" t="s">
@@ -2104,7 +2099,7 @@
       <c r="C44" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" t="s">
         <v>55</v>
       </c>
       <c r="E44" t="s">
@@ -2136,7 +2131,7 @@
       <c r="C45" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" t="s">
         <v>55</v>
       </c>
       <c r="E45" t="s">
@@ -2168,7 +2163,7 @@
       <c r="C46" t="s">
         <v>85</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" t="s">
         <v>55</v>
       </c>
       <c r="E46" t="s">
@@ -2200,7 +2195,7 @@
       <c r="C47" t="s">
         <v>85</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" t="s">
         <v>55</v>
       </c>
       <c r="E47" t="s">
@@ -2232,7 +2227,7 @@
       <c r="C48" t="s">
         <v>85</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" t="s">
         <v>55</v>
       </c>
       <c r="E48" t="s">
@@ -2264,7 +2259,7 @@
       <c r="C49" t="s">
         <v>85</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" t="s">
         <v>55</v>
       </c>
       <c r="E49" t="s">
@@ -2296,7 +2291,7 @@
       <c r="C50" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" t="s">
         <v>75</v>
       </c>
       <c r="E50" t="s">
@@ -2328,7 +2323,7 @@
       <c r="C51" t="s">
         <v>87</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" t="s">
         <v>44</v>
       </c>
       <c r="E51" t="s">
@@ -2364,7 +2359,7 @@
       <c r="C52" t="s">
         <v>87</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" t="s">
         <v>47</v>
       </c>
       <c r="E52" t="s">
@@ -2400,7 +2395,7 @@
       <c r="C53" t="s">
         <v>87</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" t="s">
         <v>77</v>
       </c>
       <c r="E53" t="s">
@@ -2436,7 +2431,7 @@
       <c r="C54" t="s">
         <v>86</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" t="s">
         <v>79</v>
       </c>
       <c r="E54" t="s">
@@ -2494,31 +2489,31 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A56" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" s="8" t="s">
+      <c r="A56" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D56" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F56" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H56" s="8">
-        <v>0</v>
-      </c>
-      <c r="I56" s="8">
+      <c r="F56" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H56" s="6">
+        <v>0</v>
+      </c>
+      <c r="I56" s="6">
         <v>2018</v>
       </c>
       <c r="J56" s="4"/>
@@ -2533,7 +2528,7 @@
       <c r="C57" t="s">
         <v>88</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E57" t="s">
@@ -2569,7 +2564,7 @@
       <c r="C58" t="s">
         <v>74</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" t="s">
         <v>74</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -2602,7 +2597,7 @@
       <c r="C59" t="s">
         <v>86</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" t="s">
         <v>75</v>
       </c>
       <c r="E59" s="3" t="s">
@@ -2637,7 +2632,7 @@
       <c r="C60" t="s">
         <v>86</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" t="s">
         <v>76</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2669,7 +2664,7 @@
       <c r="C61" t="s">
         <v>86</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" t="s">
         <v>79</v>
       </c>
       <c r="E61" s="3" t="s">
@@ -2704,7 +2699,7 @@
       <c r="C62" t="s">
         <v>84</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" t="s">
         <v>78</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2736,7 +2731,7 @@
       <c r="C63" t="s">
         <v>84</v>
       </c>
-      <c r="D63" s="6"/>
+      <c r="D63" s="3"/>
       <c r="E63" s="3" t="s">
         <v>10</v>
       </c>
@@ -2766,7 +2761,7 @@
       <c r="C64" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="6"/>
+      <c r="D64" s="3"/>
       <c r="E64" s="3" t="s">
         <v>12</v>
       </c>
@@ -2797,7 +2792,7 @@
       <c r="C65" t="s">
         <v>87</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" t="s">
         <v>44</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2832,7 +2827,7 @@
       <c r="C66" t="s">
         <v>87</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" t="s">
         <v>47</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2844,7 +2839,7 @@
       <c r="G66" t="s">
         <v>6</v>
       </c>
-      <c r="H66" s="10">
+      <c r="H66" s="7">
         <f>34/4</f>
         <v>8.5</v>
       </c>
@@ -2868,7 +2863,7 @@
       <c r="C67" t="s">
         <v>87</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" t="s">
         <v>77</v>
       </c>
       <c r="E67" s="3" t="s">
@@ -2900,7 +2895,7 @@
       <c r="C68" t="s">
         <v>88</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E68" s="3" t="s">
@@ -2936,7 +2931,7 @@
       <c r="C69" t="s">
         <v>85</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" t="s">
         <v>54</v>
       </c>
       <c r="E69" s="3" t="s">
@@ -2965,7 +2960,7 @@
       <c r="C70" t="s">
         <v>85</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" t="s">
         <v>55</v>
       </c>
       <c r="E70" s="3" t="s">
@@ -3000,7 +2995,7 @@
       <c r="C71" t="s">
         <v>74</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" t="s">
         <v>74</v>
       </c>
       <c r="E71" s="3" t="s">
@@ -3033,7 +3028,7 @@
       <c r="C72" t="s">
         <v>86</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" t="s">
         <v>75</v>
       </c>
       <c r="E72" s="3" t="s">
@@ -3069,7 +3064,7 @@
       <c r="C73" t="s">
         <v>86</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" t="s">
         <v>76</v>
       </c>
       <c r="E73" s="3" t="s">
@@ -3101,7 +3096,7 @@
       <c r="C74" t="s">
         <v>86</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" t="s">
         <v>79</v>
       </c>
       <c r="E74" s="3" t="s">
@@ -3137,7 +3132,7 @@
       <c r="C75" t="s">
         <v>84</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" t="s">
         <v>78</v>
       </c>
       <c r="E75" s="3" t="s">
@@ -3198,7 +3193,7 @@
       <c r="C77" t="s">
         <v>84</v>
       </c>
-      <c r="D77" s="6"/>
+      <c r="D77" s="3"/>
       <c r="E77" s="3" t="s">
         <v>12</v>
       </c>
@@ -3228,7 +3223,7 @@
       <c r="C78" t="s">
         <v>87</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" t="s">
         <v>44</v>
       </c>
       <c r="E78" s="3" t="s">
@@ -3260,7 +3255,7 @@
       <c r="C79" t="s">
         <v>87</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" t="s">
         <v>47</v>
       </c>
       <c r="E79" s="3" t="s">
@@ -3292,7 +3287,7 @@
       <c r="C80" t="s">
         <v>87</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" t="s">
         <v>77</v>
       </c>
       <c r="E80" s="3" t="s">
@@ -3325,7 +3320,7 @@
       <c r="C81" t="s">
         <v>88</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E81" s="3" t="s">
@@ -3358,7 +3353,7 @@
       <c r="C82" t="s">
         <v>85</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" t="s">
         <v>54</v>
       </c>
       <c r="E82" s="3" t="s">
@@ -3391,7 +3386,7 @@
       <c r="C83" t="s">
         <v>85</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" t="s">
         <v>55</v>
       </c>
       <c r="E83" s="3" t="s">
@@ -3438,15 +3433,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <VITOOpportunity xmlns="140ef148-925d-4328-9f08-4c558858642d" xsi:nil="true"/>
@@ -3465,7 +3451,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008656C54434DC964B8FD3868A8B66F29D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4cd58309bee83cc2fddaf7c13d6b5907">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="140ef148-925d-4328-9f08-4c558858642d" xmlns:ns3="6c5eb39b-f36b-40ff-b18f-c0876d3e7216" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffcd0c1f2f7d4c34e5fd067233c8c98a" ns2:_="" ns3:_="">
     <xsd:import namespace="140ef148-925d-4328-9f08-4c558858642d"/>
@@ -3770,15 +3756,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC14FB36-EC2D-401D-A6EC-CDE3DC565261}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFEC446D-31D9-4495-8D2E-CCE4FDE20A1B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3789,7 +3776,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE36D835-F73B-4235-B216-4C08381BAE1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3806,4 +3793,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC14FB36-EC2D-401D-A6EC-CDE3DC565261}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>